<commit_message>
Downgraded to release version
</commit_message>
<xml_diff>
--- a/inst/extdata/bu/mk/AAA_f18_text_temp.xlsx
+++ b/inst/extdata/bu/mk/AAA_f18_text_temp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rprojects\eamenaR\inst\extdata\bu\mk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rprojects\eamena-arches-dev\data\bulk\bu\mk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E470D722-5671-4F65-A8E8-77679207E2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3D69DAB-3CA0-46D9-9D08-7CA4D026A2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="71">
   <si>
     <t>AAA_Description_French</t>
   </si>
@@ -377,18 +377,6 @@
   </si>
   <si>
     <t>Point</t>
-  </si>
-  <si>
-    <t>Dam</t>
-  </si>
-  <si>
-    <t>Borne</t>
-  </si>
-  <si>
-    <t>Quelques pierres</t>
-  </si>
-  <si>
-    <t>Quarry</t>
   </si>
 </sst>
 </file>
@@ -828,13 +816,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL13"/>
+  <dimension ref="A1:AH13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S2" sqref="S2"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -844,7 +832,7 @@
     <col min="11" max="11" width="94.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="6" customFormat="1" ht="31.95" customHeight="1" thickBot="1">
+    <row r="1" spans="1:34" s="6" customFormat="1" ht="31.95" customHeight="1" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -897,70 +885,58 @@
         <v>10</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="W1" s="6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="X1" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="Y1" s="6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="Z1" s="6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="AD1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="AE1" s="6" t="s">
-        <v>20</v>
-      </c>
       <c r="AF1" s="6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="AG1" s="6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="AH1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="AI1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="AJ1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="AK1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="AL1" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="265.8" thickBot="1">
+    <row r="2" spans="1:34" ht="265.8" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
@@ -995,14 +971,14 @@
       <c r="M2" s="11" t="s">
         <v>27</v>
       </c>
+      <c r="U2" s="10" t="s">
+        <v>27</v>
+      </c>
       <c r="Y2" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="AC2" s="10" t="s">
-        <v>27</v>
-      </c>
     </row>
-    <row r="3" spans="1:38" ht="31.8" thickBot="1">
+    <row r="3" spans="1:34" ht="31.8" thickBot="1">
       <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
@@ -1035,7 +1011,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="34.799999999999997" thickBot="1">
+    <row r="4" spans="1:34" ht="34.799999999999997" thickBot="1">
       <c r="A4" s="1" t="s">
         <v>43</v>
       </c>
@@ -1068,7 +1044,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="31.8" thickBot="1">
+    <row r="5" spans="1:34" ht="31.8" thickBot="1">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -1103,9 +1079,9 @@
       <c r="M5" t="s">
         <v>27</v>
       </c>
-      <c r="AE5" s="7"/>
+      <c r="AA5" s="7"/>
     </row>
-    <row r="6" spans="1:38" ht="31.8" thickBot="1">
+    <row r="6" spans="1:34" ht="31.8" thickBot="1">
       <c r="A6" s="1" t="s">
         <v>45</v>
       </c>
@@ -1144,7 +1120,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:38" ht="16.2" thickBot="1">
+    <row r="7" spans="1:34" ht="16.2" thickBot="1">
       <c r="A7" s="1" t="s">
         <v>46</v>
       </c>
@@ -1180,7 +1156,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:38" ht="94.2" thickBot="1">
+    <row r="8" spans="1:34" ht="94.2" thickBot="1">
       <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
@@ -1212,11 +1188,11 @@
       <c r="K8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="X8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:38" ht="97.2" thickBot="1">
+    <row r="9" spans="1:34" ht="97.2" thickBot="1">
       <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
@@ -1252,7 +1228,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:38" ht="19.2" thickBot="1">
+    <row r="10" spans="1:34" ht="19.2" thickBot="1">
       <c r="A10" s="1" t="s">
         <v>49</v>
       </c>
@@ -1288,7 +1264,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="34.799999999999997" thickBot="1">
+    <row r="11" spans="1:34" ht="34.799999999999997" thickBot="1">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
@@ -1324,7 +1300,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:38" ht="31.8" thickBot="1">
+    <row r="12" spans="1:34" ht="31.8" thickBot="1">
       <c r="A12" s="1" t="s">
         <v>51</v>
       </c>
@@ -1360,7 +1336,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:38" ht="34.799999999999997" thickBot="1">
+    <row r="13" spans="1:34" ht="34.799999999999997" thickBot="1">
       <c r="A13" s="1" t="s">
         <v>52</v>
       </c>

</xml_diff>